<commit_message>
3675: Fixed extra zero at end of number
</commit_message>
<xml_diff>
--- a/spec/fixtures/user_batches/varying_info.xlsx
+++ b/spec/fixtures/user_batches/varying_info.xlsx
@@ -18,8 +18,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Thomas Smyth</author>
+  </authors>
+  <commentList>
+    <comment ref="C4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Thomas Smyth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This one is a number so we are sure it can handle numbers.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Username</t>
   </si>
@@ -61,9 +95,6 @@
   </si>
   <si>
     <t>Flim Flo</t>
-  </si>
-  <si>
-    <t>+2236366363</t>
   </si>
   <si>
     <t>f@fl.com</t>
@@ -100,7 +131,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -133,6 +164,27 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,11 +204,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -168,8 +223,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -499,14 +558,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
@@ -530,7 +592,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
@@ -565,44 +627,44 @@
       <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>14</v>
+      <c r="C4" s="7">
+        <v>123456789</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="4"/>
       <c r="E5" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="F6" s="4"/>
     </row>
@@ -615,6 +677,8 @@
     <hyperlink ref="E6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId6"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
874: User batch changes for new fields
</commit_message>
<xml_diff>
--- a/spec/fixtures/user_batches/varying_info.xlsx
+++ b/spec/fixtures/user_batches/varying_info.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bertonma/programming/sassafras/elmo/spec/fixtures/user_batches/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -53,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Username</t>
   </si>
@@ -125,6 +133,33 @@
   </si>
   <si>
     <t>a.bob</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Birth Year</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>Man</t>
+  </si>
+  <si>
+    <t>Woman</t>
+  </si>
+  <si>
+    <t>Genderqueer</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>1989</t>
+  </si>
+  <si>
+    <t>Unknown Region</t>
   </si>
 </sst>
 </file>
@@ -234,6 +269,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -559,18 +599,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,13 +628,22 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -601,12 +654,17 @@
         <v>7</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -615,12 +673,19 @@
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -631,12 +696,19 @@
         <v>123456789</v>
       </c>
       <c r="D4" s="5"/>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -645,12 +717,17 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -663,26 +740,24 @@
       <c r="D6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="I6" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H4" r:id="rId3"/>
+    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="H6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId6"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
9127: Add spec for error cutoff
</commit_message>
<xml_diff>
--- a/spec/fixtures/user_batches/varying_info.xlsx
+++ b/spec/fixtures/user_batches/varying_info.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bertonma/programming/sassafras/elmo/spec/fixtures/user_batches/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomsmyth/code/nemo/spec/fixtures/user_batches/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -239,9 +239,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -260,10 +261,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -602,7 +604,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>